<commit_message>
added the Sprint3 Code
</commit_message>
<xml_diff>
--- a/src/main/resources/Book1.xlsx
+++ b/src/main/resources/Book1.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>TestCase</t>
   </si>
@@ -463,7 +463,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>

</xml_diff>